<commit_message>
Created sprintstories for the coming 2 weeks. Divided backog story F2 into more scalable sprintstories.
</commit_message>
<xml_diff>
--- a/stories/stories.xlsx
+++ b/stories/stories.xlsx
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added sfGuardPlugin, extended model with relation user <-> sfGuard, added first test scripts.
</commit_message>
<xml_diff>
--- a/stories/stories.xlsx
+++ b/stories/stories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -106,9 +106,6 @@
     <t>F2: Show personal load</t>
   </si>
   <si>
-    <t xml:space="preserve">F2 : Make login </t>
-  </si>
-  <si>
     <t>Make a login system for user. There are to type of users : customer en transporter. Both see different starting pages.</t>
   </si>
   <si>
@@ -121,19 +118,28 @@
     <t>A customer and transporter can log in to the system.</t>
   </si>
   <si>
-    <t>F2: Register user</t>
-  </si>
-  <si>
     <t>A user can register as a customer or a a transporter  The adminstrator has to approve the user to log in.</t>
   </si>
   <si>
-    <t>F2: Edit/Show Customer detail</t>
-  </si>
-  <si>
-    <t>F2: Edit/Show Transporter detail</t>
-  </si>
-  <si>
     <t>wip</t>
+  </si>
+  <si>
+    <t>hans</t>
+  </si>
+  <si>
+    <t>eric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F7 : Make login </t>
+  </si>
+  <si>
+    <t>F7: Edit/Show Customer detail</t>
+  </si>
+  <si>
+    <t>F7: Edit/Show Transporter detail</t>
+  </si>
+  <si>
+    <t>F7: Register user</t>
   </si>
 </sst>
 </file>
@@ -640,7 +646,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -705,12 +711,14 @@
       <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="105">
@@ -727,7 +735,9 @@
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="30">
@@ -742,9 +752,11 @@
         <v>40</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="60">
@@ -761,12 +773,15 @@
       <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="45">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4">
         <v>50</v>
@@ -775,15 +790,17 @@
         <v>70</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="45">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C8" s="4">
         <v>70</v>
@@ -792,15 +809,17 @@
         <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="30">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" s="4">
         <v>70</v>
@@ -809,7 +828,7 @@
         <v>50</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="1"/>
@@ -817,7 +836,7 @@
     <row r="10" spans="1:8" ht="30">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="4">
         <v>70</v>
@@ -826,7 +845,7 @@
         <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="1"/>

</xml_diff>